<commit_message>
se crea una rama feature/cine_carga_datos excell
</commit_message>
<xml_diff>
--- a/bd_cine_colombia/data/data_for_loading.xlsx
+++ b/bd_cine_colombia/data/data_for_loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCC\UCC_CreacionBD\bd_cinecolombia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repositorio\ucc-creacionBD\cine_carga_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2F0A4A-6217-4529-A7BC-8844E872AA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52794D2C-D92F-4820-8D2B-236581DD62EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{42B65FB2-2B7F-49E6-A427-49DEDB5C9C54}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{42B65FB2-2B7F-49E6-A427-49DEDB5C9C54}"/>
   </bookViews>
   <sheets>
     <sheet name="PAIS" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="1023">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -3116,193 +3116,16 @@
     <t>Puerto Carreño</t>
   </si>
   <si>
-    <t>Ama</t>
-  </si>
-  <si>
-    <t>Ant</t>
-  </si>
-  <si>
-    <t>Ara</t>
-  </si>
-  <si>
-    <t>Atl</t>
-  </si>
-  <si>
-    <t>Bog</t>
-  </si>
-  <si>
-    <t>Bol</t>
-  </si>
-  <si>
-    <t>Boy</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Caq</t>
-  </si>
-  <si>
-    <t>Cas</t>
-  </si>
-  <si>
-    <t>Cau</t>
-  </si>
-  <si>
-    <t>Ces</t>
-  </si>
-  <si>
-    <t>Cho</t>
-  </si>
-  <si>
-    <t>Cór</t>
-  </si>
-  <si>
-    <t>Cun</t>
-  </si>
-  <si>
-    <t>Gua</t>
-  </si>
-  <si>
-    <t>Guv</t>
-  </si>
-  <si>
-    <t>Hui</t>
-  </si>
-  <si>
-    <t>LaG</t>
-  </si>
-  <si>
-    <t>Mag</t>
-  </si>
-  <si>
-    <t>Met</t>
-  </si>
-  <si>
-    <t>Nar</t>
-  </si>
-  <si>
-    <t>Nsa</t>
-  </si>
-  <si>
-    <t>Put</t>
-  </si>
-  <si>
-    <t>Qui</t>
-  </si>
-  <si>
-    <t>Ris</t>
-  </si>
-  <si>
-    <t>Sap</t>
-  </si>
-  <si>
-    <t>San</t>
-  </si>
-  <si>
-    <t>Suc</t>
-  </si>
-  <si>
-    <t>Tol</t>
-  </si>
-  <si>
-    <t>Vac</t>
-  </si>
-  <si>
-    <t>Vau</t>
-  </si>
-  <si>
-    <t>Vic</t>
-  </si>
-  <si>
     <t>ID_dep</t>
   </si>
   <si>
     <t>Ciudad_Capital</t>
   </si>
   <si>
-    <t>Let</t>
-  </si>
-  <si>
-    <t>Med</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Cart</t>
-  </si>
-  <si>
-    <t>Tun</t>
-  </si>
-  <si>
-    <t>Man</t>
-  </si>
-  <si>
-    <t>Flo</t>
-  </si>
-  <si>
-    <t>Yop</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>Vap</t>
-  </si>
-  <si>
-    <t>Qd</t>
-  </si>
-  <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Iní</t>
-  </si>
-  <si>
-    <t>SJG</t>
-  </si>
-  <si>
-    <t>Nei</t>
-  </si>
-  <si>
-    <t>Rio</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Viv</t>
-  </si>
-  <si>
-    <t>Pas</t>
-  </si>
-  <si>
-    <t>Moc</t>
-  </si>
-  <si>
-    <t>Arm</t>
-  </si>
-  <si>
-    <t>Per</t>
-  </si>
-  <si>
-    <t>Sad</t>
-  </si>
-  <si>
-    <t>Buc</t>
-  </si>
-  <si>
-    <t>Sinc</t>
-  </si>
-  <si>
-    <t>Iba</t>
-  </si>
-  <si>
-    <t>Mit</t>
-  </si>
-  <si>
-    <t>Ptc</t>
+    <t xml:space="preserve"> Cúcuta</t>
+  </si>
+  <si>
+    <t>Agua de dios</t>
   </si>
 </sst>
 </file>
@@ -3461,7 +3284,7 @@
     <tableColumn id="2" xr3:uid="{C602A8A4-9852-41B4-9E7A-BC04172E43A1}" uniqueName="2" name="Capital" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{B331BE2D-ECF4-471C-A1D7-46A7419ACA2C}" uniqueName="3" name="ID_dep" queryTableFieldId="3" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{E66CE48E-8C7D-4D46-9FDA-D72D5C59C600}" uniqueName="4" name="SCRIPT" queryTableFieldId="4" dataDxfId="4">
-      <calculatedColumnFormula>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</calculatedColumnFormula>
+      <calculatedColumnFormula>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3782,18 +3605,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95853DF-D41B-4F39-9D29-ADB9D9D0BAD2}">
   <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.296875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3810,7 +3633,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3828,7 +3651,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AFG', 'Afghanistan', '93');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3846,7 +3669,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ALB', 'Albania', '355');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3864,7 +3687,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DZA', 'Algeria', '213');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3882,7 +3705,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ASM', 'American Samoa', '1-684');</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3900,7 +3723,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AND', 'Andorra', '376');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3918,7 +3741,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AGO', 'Angola', '244');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3936,7 +3759,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AIA', 'Anguilla', '1-264');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3954,7 +3777,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ATA', 'Antarctica', '672');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -3972,7 +3795,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ATG', 'Antigua and Barbuda', '1-268');</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3990,7 +3813,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ARG', 'Argentina', '54');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -4008,7 +3831,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ARM', 'Armenia', '374');</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -4026,7 +3849,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ABW', 'Aruba', '297');</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -4044,7 +3867,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AUS', 'Australia', '61');</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4062,7 +3885,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AUT', 'Austria', '43');</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -4080,7 +3903,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('AZE', 'Azerbaijan', '994');</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -4098,7 +3921,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BHS', 'Bahamas', '1-242');</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -4116,7 +3939,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BHR', 'Bahrain', '973');</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -4134,7 +3957,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BGD', 'Bangladesh', '880');</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -4152,7 +3975,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BRB', 'Barbados', '1-246');</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -4170,7 +3993,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BLR', 'Belarus', '375');</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -4188,7 +4011,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BEL', 'Belgium', '32');</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -4206,7 +4029,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BLZ', 'Belize', '501');</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -4224,7 +4047,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BEN', 'Benin', '229');</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -4242,7 +4065,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BMU', 'Bermuda', '1-441');</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -4260,7 +4083,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BTN', 'Bhutan', '975');</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -4278,7 +4101,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BOL', 'Bolivia', '591');</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -4296,7 +4119,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BIH', 'Bosnia and Herzegovina', '387');</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -4314,7 +4137,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BWA', 'Botswana', '267');</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -4332,7 +4155,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BRA', 'Brazil', '55');</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -4350,7 +4173,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IOT', 'British Indian Ocean Territory', '246');</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -4368,7 +4191,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VGB', 'British Virgin Islands', '1-284');</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -4386,7 +4209,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BRN', 'Brunei', '673');</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -4404,7 +4227,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BGR', 'Bulgaria', '359');</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -4422,7 +4245,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BFA', 'Burkina Faso', '226');</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -4440,7 +4263,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BDI', 'Burundi', '257');</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4458,7 +4281,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KHM', 'Cambodia', '855');</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -4476,7 +4299,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CMR', 'Cameroon', '237');</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4494,7 +4317,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CAN', 'Canada', '1');</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>156</v>
       </c>
@@ -4512,7 +4335,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CPV', 'Cape Verde', '238');</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>160</v>
       </c>
@@ -4530,7 +4353,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CYM', 'Cayman Islands', '1-345');</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>164</v>
       </c>
@@ -4548,7 +4371,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CAF', 'Central African Republic', '236');</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>168</v>
       </c>
@@ -4566,7 +4389,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TCD', 'Chad', '235');</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -4584,7 +4407,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CHL', 'Chile', '56');</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -4602,7 +4425,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CHN', 'China', '86');</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>180</v>
       </c>
@@ -4620,7 +4443,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CXR', 'Christmas Island', '61');</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>183</v>
       </c>
@@ -4638,7 +4461,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CCK', 'Cocos Islands', '61');</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>186</v>
       </c>
@@ -4656,7 +4479,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('COL', 'Colombia', '57');</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -4674,7 +4497,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('COM', 'Comoros', '269');</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>194</v>
       </c>
@@ -4692,7 +4515,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('COK', 'Cook Islands', '682');</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>198</v>
       </c>
@@ -4710,7 +4533,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CRI', 'Costa Rica', '506');</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>202</v>
       </c>
@@ -4728,7 +4551,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('HRV', 'Croatia', '385');</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -4746,7 +4569,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CUB', 'Cuba', '53');</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>210</v>
       </c>
@@ -4764,7 +4587,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CUW', 'Curacao', '599');</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>214</v>
       </c>
@@ -4782,7 +4605,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CYP', 'Cyprus', '357');</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>218</v>
       </c>
@@ -4800,7 +4623,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CZE', 'Czech Republic', '420');</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -4818,7 +4641,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('COD', 'Democratic Republic of the Congo', '243');</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>226</v>
       </c>
@@ -4836,7 +4659,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DNK', 'Denmark', '45');</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>230</v>
       </c>
@@ -4854,7 +4677,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DJI', 'Djibouti', '253');</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>234</v>
       </c>
@@ -4872,7 +4695,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DMA', 'Dominica', '1-767');</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>238</v>
       </c>
@@ -4890,7 +4713,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DOM', 'Dominican Republic', '1-809, 1-829, 1-849');</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>242</v>
       </c>
@@ -4908,7 +4731,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TLS', 'East Timor', '670');</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>246</v>
       </c>
@@ -4926,7 +4749,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ECU', 'Ecuador', '593');</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>250</v>
       </c>
@@ -4944,7 +4767,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('EGY', 'Egypt', '20');</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>254</v>
       </c>
@@ -4962,7 +4785,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SLV', 'El Salvador', '503');</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>258</v>
       </c>
@@ -4980,7 +4803,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GNQ', 'Equatorial Guinea', '240');</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>262</v>
       </c>
@@ -4998,7 +4821,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ERI', 'Eritrea', '291');</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>266</v>
       </c>
@@ -5016,7 +4839,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('EST', 'Estonia', '372');</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>270</v>
       </c>
@@ -5034,7 +4857,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ETH', 'Ethiopia', '251');</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>274</v>
       </c>
@@ -5052,7 +4875,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FLK', 'Falkland Islands', '500');</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>278</v>
       </c>
@@ -5070,7 +4893,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FRO', 'Faroe Islands', '298');</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>282</v>
       </c>
@@ -5088,7 +4911,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FJI', 'Fiji', '679');</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>286</v>
       </c>
@@ -5106,7 +4929,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FIN', 'Finland', '358');</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>290</v>
       </c>
@@ -5124,7 +4947,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FRA', 'France', '33');</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>294</v>
       </c>
@@ -5142,7 +4965,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PYF', 'French Polynesia', '689');</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>298</v>
       </c>
@@ -5160,7 +4983,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GAB', 'Gabon', '241');</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>302</v>
       </c>
@@ -5178,7 +5001,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GMB', 'Gambia', '220');</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>306</v>
       </c>
@@ -5196,7 +5019,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GEO', 'Georgia', '995');</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>310</v>
       </c>
@@ -5214,7 +5037,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('DEU', 'Germany', '49');</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>314</v>
       </c>
@@ -5232,7 +5055,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GHA', 'Ghana', '233');</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>318</v>
       </c>
@@ -5250,7 +5073,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GIB', 'Gibraltar', '350');</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>322</v>
       </c>
@@ -5268,7 +5091,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GRC', 'Greece', '30');</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>326</v>
       </c>
@@ -5286,7 +5109,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GRL', 'Greenland', '299');</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>330</v>
       </c>
@@ -5304,7 +5127,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GRD', 'Grenada', '1-473');</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>334</v>
       </c>
@@ -5322,7 +5145,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GUM', 'Guam', '1-671');</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>338</v>
       </c>
@@ -5340,7 +5163,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GTM', 'Guatemala', '502');</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>342</v>
       </c>
@@ -5358,7 +5181,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GGY', 'Guernsey', '44-1481');</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>346</v>
       </c>
@@ -5376,7 +5199,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GIN', 'Guinea', '224');</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>350</v>
       </c>
@@ -5394,7 +5217,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GNB', 'Guinea-Bissau', '245');</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>354</v>
       </c>
@@ -5412,7 +5235,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GUY', 'Guyana', '592');</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>358</v>
       </c>
@@ -5430,7 +5253,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('HTI', 'Haiti', '509');</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>362</v>
       </c>
@@ -5448,7 +5271,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('HND', 'Honduras', '504');</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>366</v>
       </c>
@@ -5466,7 +5289,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('HKG', 'Hong Kong', '852');</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>370</v>
       </c>
@@ -5484,7 +5307,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('HUN', 'Hungary', '36');</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>374</v>
       </c>
@@ -5502,7 +5325,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ISL', 'Iceland', '354');</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>378</v>
       </c>
@@ -5520,7 +5343,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IND', 'India', '91');</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>382</v>
       </c>
@@ -5538,7 +5361,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IDN', 'Indonesia', '62');</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>386</v>
       </c>
@@ -5556,7 +5379,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IRN', 'Iran', '98');</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>390</v>
       </c>
@@ -5574,7 +5397,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IRQ', 'Iraq', '964');</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>394</v>
       </c>
@@ -5592,7 +5415,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IRL', 'Ireland', '353');</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>398</v>
       </c>
@@ -5610,7 +5433,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('IMN', 'Isle of Man', '44-1624');</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>402</v>
       </c>
@@ -5628,7 +5451,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ISR', 'Israel', '972');</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>406</v>
       </c>
@@ -5646,7 +5469,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ITA', 'Italy', '39');</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>410</v>
       </c>
@@ -5664,7 +5487,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CIV', 'Ivory Coast', '225');</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>414</v>
       </c>
@@ -5682,7 +5505,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('JAM', 'Jamaica', '1-876');</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>418</v>
       </c>
@@ -5700,7 +5523,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('JPN', 'Japan', '81');</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>422</v>
       </c>
@@ -5718,7 +5541,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('JEY', 'Jersey', '44-1534');</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>426</v>
       </c>
@@ -5736,7 +5559,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('JOR', 'Jordan', '962');</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>430</v>
       </c>
@@ -5754,7 +5577,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KAZ', 'Kazakhstan', '7');</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>434</v>
       </c>
@@ -5772,7 +5595,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KEN', 'Kenya', '254');</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>438</v>
       </c>
@@ -5790,7 +5613,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KIR', 'Kiribati', '686');</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>442</v>
       </c>
@@ -5808,7 +5631,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('XKX', 'Kosovo', '383');</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>446</v>
       </c>
@@ -5826,7 +5649,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KWT', 'Kuwait', '965');</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>450</v>
       </c>
@@ -5844,7 +5667,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KGZ', 'Kyrgyzstan', '996');</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>454</v>
       </c>
@@ -5862,7 +5685,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LAO', 'Laos', '856');</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>458</v>
       </c>
@@ -5880,7 +5703,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LVA', 'Latvia', '371');</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>462</v>
       </c>
@@ -5898,7 +5721,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LBN', 'Lebanon', '961');</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>466</v>
       </c>
@@ -5916,7 +5739,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LSO', 'Lesotho', '266');</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>470</v>
       </c>
@@ -5934,7 +5757,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LBR', 'Liberia', '231');</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>474</v>
       </c>
@@ -5952,7 +5775,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LBY', 'Libya', '218');</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>478</v>
       </c>
@@ -5970,7 +5793,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LIE', 'Liechtenstein', '423');</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>482</v>
       </c>
@@ -5988,7 +5811,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LTU', 'Lithuania', '370');</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>486</v>
       </c>
@@ -6006,7 +5829,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LUX', 'Luxembourg', '352');</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>490</v>
       </c>
@@ -6024,7 +5847,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MAC', 'Macau', '853');</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>494</v>
       </c>
@@ -6042,7 +5865,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MKD', 'Macedonia', '389');</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>498</v>
       </c>
@@ -6060,7 +5883,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MDG', 'Madagascar', '261');</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>502</v>
       </c>
@@ -6078,7 +5901,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MWI', 'Malawi', '265');</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>506</v>
       </c>
@@ -6096,7 +5919,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MYS', 'Malaysia', '60');</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>510</v>
       </c>
@@ -6114,7 +5937,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MDV', 'Maldives', '960');</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>514</v>
       </c>
@@ -6132,7 +5955,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MLI', 'Mali', '223');</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>518</v>
       </c>
@@ -6150,7 +5973,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MLT', 'Malta', '356');</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>522</v>
       </c>
@@ -6168,7 +5991,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MHL', 'Marshall Islands', '692');</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>526</v>
       </c>
@@ -6186,7 +6009,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MRT', 'Mauritania', '222');</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>530</v>
       </c>
@@ -6204,7 +6027,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MUS', 'Mauritius', '230');</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>534</v>
       </c>
@@ -6222,7 +6045,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MYT', 'Mayotte', '262');</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>538</v>
       </c>
@@ -6240,7 +6063,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MEX', 'Mexico', '52');</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>542</v>
       </c>
@@ -6258,7 +6081,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('FSM', 'Micronesia', '691');</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>546</v>
       </c>
@@ -6276,7 +6099,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MDA', 'Moldova', '373');</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>550</v>
       </c>
@@ -6294,7 +6117,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MCO', 'Monaco', '377');</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>554</v>
       </c>
@@ -6312,7 +6135,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MNG', 'Mongolia', '976');</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>558</v>
       </c>
@@ -6330,7 +6153,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MNE', 'Montenegro', '382');</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>562</v>
       </c>
@@ -6348,7 +6171,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MSR', 'Montserrat', '1-664');</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>566</v>
       </c>
@@ -6366,7 +6189,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MAR', 'Morocco', '212');</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>570</v>
       </c>
@@ -6384,7 +6207,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MOZ', 'Mozambique', '258');</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>574</v>
       </c>
@@ -6402,7 +6225,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MMR', 'Myanmar', '95');</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>578</v>
       </c>
@@ -6420,7 +6243,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NAM', 'Namibia', '264');</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>582</v>
       </c>
@@ -6438,7 +6261,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NRU', 'Nauru', '674');</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>586</v>
       </c>
@@ -6456,7 +6279,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NPL', 'Nepal', '977');</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>590</v>
       </c>
@@ -6474,7 +6297,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NLD', 'Netherlands', '31');</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>594</v>
       </c>
@@ -6492,7 +6315,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ANT', 'Netherlands Antilles', '599');</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>597</v>
       </c>
@@ -6510,7 +6333,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NCL', 'New Caledonia', '687');</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>601</v>
       </c>
@@ -6528,7 +6351,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NZL', 'New Zealand', '64');</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>605</v>
       </c>
@@ -6546,7 +6369,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NIC', 'Nicaragua', '505');</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>609</v>
       </c>
@@ -6564,7 +6387,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NER', 'Niger', '227');</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>613</v>
       </c>
@@ -6582,7 +6405,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NGA', 'Nigeria', '234');</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>617</v>
       </c>
@@ -6600,7 +6423,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NIU', 'Niue', '683');</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>621</v>
       </c>
@@ -6618,7 +6441,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PRK', 'North Korea', '850');</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>625</v>
       </c>
@@ -6636,7 +6459,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MNP', 'Northern Mariana Islands', '1-670');</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>629</v>
       </c>
@@ -6654,7 +6477,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('NOR', 'Norway', '47');</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>633</v>
       </c>
@@ -6672,7 +6495,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('OMN', 'Oman', '968');</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>637</v>
       </c>
@@ -6690,7 +6513,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PAK', 'Pakistan', '92');</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>641</v>
       </c>
@@ -6708,7 +6531,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PLW', 'Palau', '680');</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>645</v>
       </c>
@@ -6726,7 +6549,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PSE', 'Palestine', '970');</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>649</v>
       </c>
@@ -6744,7 +6567,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PAN', 'Panama', '507');</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>653</v>
       </c>
@@ -6762,7 +6585,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PNG', 'Papua New Guinea', '675');</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>657</v>
       </c>
@@ -6780,7 +6603,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PRY', 'Paraguay', '595');</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>661</v>
       </c>
@@ -6798,7 +6621,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PER', 'Peru', '51');</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>665</v>
       </c>
@@ -6816,7 +6639,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PHL', 'Philippines', '63');</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>669</v>
       </c>
@@ -6834,7 +6657,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PCN', 'Pitcairn', '64');</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>672</v>
       </c>
@@ -6852,7 +6675,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('POL', 'Poland', '48');</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>676</v>
       </c>
@@ -6870,7 +6693,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PRT', 'Portugal', '351');</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>680</v>
       </c>
@@ -6888,7 +6711,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('PRI', 'Puerto Rico', '1-787, 1-939');</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>684</v>
       </c>
@@ -6906,7 +6729,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('QAT', 'Qatar', '974');</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>688</v>
       </c>
@@ -6924,7 +6747,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('COG', 'Republic of the Congo', '242');</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>692</v>
       </c>
@@ -6942,7 +6765,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('REU', 'Reunion', '262');</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>695</v>
       </c>
@@ -6960,7 +6783,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ROU', 'Romania', '40');</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>699</v>
       </c>
@@ -6978,7 +6801,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('RUS', 'Russia', '7');</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>702</v>
       </c>
@@ -6996,7 +6819,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('RWA', 'Rwanda', '250');</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>706</v>
       </c>
@@ -7014,7 +6837,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('BLM', 'Saint Barthelemy', '590');</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>710</v>
       </c>
@@ -7032,7 +6855,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SHN', 'Saint Helena', '290');</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>714</v>
       </c>
@@ -7050,7 +6873,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KNA', 'Saint Kitts and Nevis', '1-869');</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>718</v>
       </c>
@@ -7068,7 +6891,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LCA', 'Saint Lucia', '1-758');</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>722</v>
       </c>
@@ -7086,7 +6909,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('MAF', 'Saint Martin', '590');</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>725</v>
       </c>
@@ -7104,7 +6927,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SPM', 'Saint Pierre and Miquelon', '508');</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>729</v>
       </c>
@@ -7122,7 +6945,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VCT', 'Saint Vincent and the Grenadines', '1-784');</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>733</v>
       </c>
@@ -7140,7 +6963,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('WSM', 'Samoa', '685');</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>737</v>
       </c>
@@ -7158,7 +6981,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SMR', 'San Marino', '378');</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>741</v>
       </c>
@@ -7176,7 +6999,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('STP', 'Sao Tome and Principe', '239');</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>745</v>
       </c>
@@ -7194,7 +7017,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SAU', 'Saudi Arabia', '966');</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>749</v>
       </c>
@@ -7212,7 +7035,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SEN', 'Senegal', '221');</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>753</v>
       </c>
@@ -7230,7 +7053,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SRB', 'Serbia', '381');</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>757</v>
       </c>
@@ -7248,7 +7071,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SYC', 'Seychelles', '248');</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>761</v>
       </c>
@@ -7266,7 +7089,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SLE', 'Sierra Leone', '232');</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>765</v>
       </c>
@@ -7284,7 +7107,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SGP', 'Singapore', '65');</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>769</v>
       </c>
@@ -7302,7 +7125,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SXM', 'Sint Maarten', '1-721');</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>773</v>
       </c>
@@ -7320,7 +7143,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SVK', 'Slovakia', '421');</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>777</v>
       </c>
@@ -7338,7 +7161,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SVN', 'Slovenia', '386');</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>781</v>
       </c>
@@ -7356,7 +7179,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SLB', 'Solomon Islands', '677');</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>785</v>
       </c>
@@ -7374,7 +7197,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SOM', 'Somalia', '252');</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>789</v>
       </c>
@@ -7392,7 +7215,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ZAF', 'South Africa', '27');</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>793</v>
       </c>
@@ -7410,7 +7233,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('KOR', 'South Korea', '82');</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>797</v>
       </c>
@@ -7428,7 +7251,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SSD', 'South Sudan', '211');</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>801</v>
       </c>
@@ -7446,7 +7269,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ESP', 'Spain', '34');</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>805</v>
       </c>
@@ -7464,7 +7287,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('LKA', 'Sri Lanka', '94');</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>809</v>
       </c>
@@ -7482,7 +7305,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SDN', 'Sudan', '249');</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>813</v>
       </c>
@@ -7500,7 +7323,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SUR', 'Suriname', '597');</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>817</v>
       </c>
@@ -7518,7 +7341,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SJM', 'Svalbard and Jan Mayen', '47');</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>820</v>
       </c>
@@ -7536,7 +7359,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SWZ', 'Swaziland', '268');</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>824</v>
       </c>
@@ -7554,7 +7377,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SWE', 'Sweden', '46');</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>828</v>
       </c>
@@ -7572,7 +7395,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('CHE', 'Switzerland', '41');</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>832</v>
       </c>
@@ -7590,7 +7413,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('SYR', 'Syria', '963');</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>836</v>
       </c>
@@ -7608,7 +7431,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TWN', 'Taiwan', '886');</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>840</v>
       </c>
@@ -7626,7 +7449,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TJK', 'Tajikistan', '992');</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>844</v>
       </c>
@@ -7644,7 +7467,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TZA', 'Tanzania', '255');</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>848</v>
       </c>
@@ -7662,7 +7485,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('THA', 'Thailand', '66');</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>852</v>
       </c>
@@ -7680,7 +7503,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TGO', 'Togo', '228');</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>856</v>
       </c>
@@ -7698,7 +7521,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TKL', 'Tokelau', '690');</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>860</v>
       </c>
@@ -7716,7 +7539,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TON', 'Tonga', '676');</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>864</v>
       </c>
@@ -7734,7 +7557,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TTO', 'Trinidad and Tobago', '1-868');</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>868</v>
       </c>
@@ -7752,7 +7575,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TUN', 'Tunisia', '216');</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>872</v>
       </c>
@@ -7770,7 +7593,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TUR', 'Turkey', '90');</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>876</v>
       </c>
@@ -7788,7 +7611,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TKM', 'Turkmenistan', '993');</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>880</v>
       </c>
@@ -7806,7 +7629,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TCA', 'Turks and Caicos Islands', '1-649');</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>884</v>
       </c>
@@ -7824,7 +7647,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('TUV', 'Tuvalu', '688');</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>888</v>
       </c>
@@ -7842,7 +7665,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VIR', 'U.S. Virgin Islands', '1-340');</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>892</v>
       </c>
@@ -7860,7 +7683,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('UGA', 'Uganda', '256');</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>896</v>
       </c>
@@ -7878,7 +7701,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('UKR', 'Ukraine', '380');</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>900</v>
       </c>
@@ -7896,7 +7719,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ARE', 'United Arab Emirates', '971');</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>904</v>
       </c>
@@ -7914,7 +7737,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('GBR', 'United Kingdom', '44');</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>908</v>
       </c>
@@ -7932,7 +7755,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('USA', 'United States', '1');</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>911</v>
       </c>
@@ -7950,7 +7773,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('URY', 'Uruguay', '598');</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>915</v>
       </c>
@@ -7968,7 +7791,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('UZB', 'Uzbekistan', '998');</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>919</v>
       </c>
@@ -7986,7 +7809,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VUT', 'Vanuatu', '678');</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>923</v>
       </c>
@@ -8004,7 +7827,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VAT', 'Vatican', '379');</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>927</v>
       </c>
@@ -8022,7 +7845,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VEN', 'Venezuela', '58');</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>931</v>
       </c>
@@ -8040,7 +7863,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('VNM', 'Vietnam', '84');</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>935</v>
       </c>
@@ -8058,7 +7881,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('WLF', 'Wallis and Futuna', '681');</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>939</v>
       </c>
@@ -8076,7 +7899,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ESH', 'Western Sahara', '212');</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>942</v>
       </c>
@@ -8094,7 +7917,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('YEM', 'Yemen', '967');</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>946</v>
       </c>
@@ -8112,7 +7935,7 @@
         <v>INSERT INTO PAIS (ID_PAIS, NOMBRE, CODIGO_TELEFONICO)VALUES ('ZMB', 'Zambia', '260');</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>950</v>
       </c>
@@ -8142,17 +7965,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6727EAFB-DED0-4134-85C0-58482A1E3CDB}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>955</v>
       </c>
@@ -8160,505 +7983,505 @@
         <v>956</v>
       </c>
       <c r="C1" t="s">
-        <v>1052</v>
+        <v>1019</v>
       </c>
       <c r="D1" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>957</v>
       </c>
       <c r="B2" t="s">
         <v>958</v>
       </c>
-      <c r="C2" t="s">
-        <v>1019</v>
+      <c r="C2">
+        <v>91</v>
       </c>
       <c r="D2" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Ama', 'COL', 'Amazonas');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('91', 'COL', 'Amazonas');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>959</v>
       </c>
       <c r="B3" t="s">
         <v>960</v>
       </c>
-      <c r="C3" t="s">
-        <v>1020</v>
+      <c r="C3">
+        <v>5</v>
       </c>
       <c r="D3" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D49&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Ant', 'COM', 'Antioquia');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('5', 'COL', 'Antioquia');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>961</v>
       </c>
       <c r="B4" t="s">
         <v>961</v>
       </c>
-      <c r="C4" t="s">
-        <v>1021</v>
+      <c r="C4">
+        <v>81</v>
       </c>
       <c r="D4" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D50&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Ara', 'COK', 'Arauca');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('81', 'COL', 'Arauca');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>962</v>
       </c>
       <c r="B5" t="s">
         <v>963</v>
       </c>
-      <c r="C5" t="s">
-        <v>1022</v>
+      <c r="C5">
+        <v>8</v>
       </c>
       <c r="D5" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D51&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Atl', 'CRI', 'Atlántico');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('8', 'COL', 'Atlántico');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>964</v>
       </c>
       <c r="B6" t="s">
         <v>964</v>
       </c>
-      <c r="C6" t="s">
-        <v>1023</v>
+      <c r="C6">
+        <v>11</v>
       </c>
       <c r="D6" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D52&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Bog', 'HRV', 'Bogotá');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('11', 'COL', 'Bogotá');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>965</v>
       </c>
       <c r="B7" t="s">
         <v>966</v>
       </c>
-      <c r="C7" t="s">
-        <v>1024</v>
+      <c r="C7">
+        <v>13</v>
       </c>
       <c r="D7" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D53&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Bol', 'CUB', 'Bolívar');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('13', 'COL', 'Bolívar');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>967</v>
       </c>
       <c r="B8" t="s">
         <v>968</v>
       </c>
-      <c r="C8" t="s">
-        <v>1025</v>
+      <c r="C8">
+        <v>15</v>
       </c>
       <c r="D8" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D54&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Boy', 'CUW', 'Boyacá');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('15', 'COL', 'Boyacá');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>969</v>
       </c>
       <c r="B9" t="s">
         <v>970</v>
       </c>
-      <c r="C9" t="s">
-        <v>1026</v>
+      <c r="C9">
+        <v>17</v>
       </c>
       <c r="D9" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D55&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cal', 'CYP', 'Caldas');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('17', 'COL', 'Caldas');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>971</v>
       </c>
       <c r="B10" t="s">
         <v>972</v>
       </c>
-      <c r="C10" t="s">
-        <v>1027</v>
+      <c r="C10">
+        <v>18</v>
       </c>
       <c r="D10" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D56&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Caq', 'CZE', 'Caquetá');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('18', 'COL', 'Caquetá');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>973</v>
       </c>
       <c r="B11" t="s">
         <v>974</v>
       </c>
-      <c r="C11" t="s">
-        <v>1028</v>
+      <c r="C11">
+        <v>85</v>
       </c>
       <c r="D11" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D57&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cas', 'COD', 'Casanare');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('85', 'COL', 'Casanare');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>975</v>
       </c>
       <c r="B12" t="s">
         <v>976</v>
       </c>
-      <c r="C12" t="s">
-        <v>1029</v>
+      <c r="C12">
+        <v>19</v>
       </c>
       <c r="D12" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D58&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cau', 'DNK', 'Cauca');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('19', 'COL', 'Cauca');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>977</v>
       </c>
       <c r="B13" t="s">
         <v>978</v>
       </c>
-      <c r="C13" t="s">
-        <v>1030</v>
+      <c r="C13">
+        <v>20</v>
       </c>
       <c r="D13" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D59&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Ces', 'DJI', 'Cesar');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('20', 'COL', 'Cesar');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>979</v>
       </c>
       <c r="B14" t="s">
         <v>980</v>
       </c>
-      <c r="C14" t="s">
-        <v>1031</v>
+      <c r="C14">
+        <v>27</v>
       </c>
       <c r="D14" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D60&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cho', 'DMA', 'Chocó');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('27', 'COL', 'Chocó');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>981</v>
       </c>
       <c r="B15" t="s">
         <v>982</v>
       </c>
-      <c r="C15" t="s">
-        <v>1032</v>
+      <c r="C15">
+        <v>23</v>
       </c>
       <c r="D15" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D61&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cór', 'DOM', 'Córdoba');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('23', 'COL', 'Córdoba');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>983</v>
       </c>
       <c r="B16" t="s">
         <v>964</v>
       </c>
-      <c r="C16" t="s">
-        <v>1033</v>
+      <c r="C16">
+        <v>25</v>
       </c>
       <c r="D16" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D62&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Cun', 'TLS', 'Cundinamarca');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('25', 'COL', 'Cundinamarca');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>984</v>
       </c>
       <c r="B17" t="s">
         <v>985</v>
       </c>
-      <c r="C17" t="s">
-        <v>1034</v>
+      <c r="C17">
+        <v>94</v>
       </c>
       <c r="D17" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D63&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Gua', 'ECU', 'Guainía');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('94', 'COL', 'Guainía');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>986</v>
       </c>
       <c r="B18" t="s">
         <v>987</v>
       </c>
-      <c r="C18" t="s">
-        <v>1035</v>
+      <c r="C18">
+        <v>95</v>
       </c>
       <c r="D18" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D64&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Guv', 'EGY', 'Guaviare');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('95', 'COL', 'Guaviare');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>988</v>
       </c>
       <c r="B19" t="s">
         <v>989</v>
       </c>
-      <c r="C19" t="s">
-        <v>1036</v>
+      <c r="C19">
+        <v>41</v>
       </c>
       <c r="D19" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D65&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Hui', 'SLV', 'Huila');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('41', 'COL', 'Huila');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>990</v>
       </c>
       <c r="B20" t="s">
         <v>991</v>
       </c>
-      <c r="C20" t="s">
-        <v>1037</v>
+      <c r="C20">
+        <v>44</v>
       </c>
       <c r="D20" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D66&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('LaG', 'GNQ', 'La Guajira');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('44', 'COL', 'La Guajira');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>992</v>
       </c>
       <c r="B21" t="s">
         <v>993</v>
       </c>
-      <c r="C21" t="s">
-        <v>1038</v>
+      <c r="C21">
+        <v>47</v>
       </c>
       <c r="D21" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D67&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Mag', 'ERI', 'Magdalena');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('47', 'COL', 'Magdalena');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>994</v>
       </c>
       <c r="B22" t="s">
         <v>995</v>
       </c>
-      <c r="C22" t="s">
-        <v>1039</v>
+      <c r="C22">
+        <v>50</v>
       </c>
       <c r="D22" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D68&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Met', 'EST', 'Meta');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('50', 'COL', 'Meta');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>996</v>
       </c>
       <c r="B23" t="s">
         <v>997</v>
       </c>
-      <c r="C23" t="s">
-        <v>1040</v>
+      <c r="C23">
+        <v>52</v>
       </c>
       <c r="D23" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D69&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Nar', 'ETH', 'Nariño');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('52', 'COL', 'Nariño');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>998</v>
       </c>
       <c r="B24" t="s">
         <v>999</v>
       </c>
-      <c r="C24" t="s">
-        <v>1041</v>
+      <c r="C24">
+        <v>54</v>
       </c>
       <c r="D24" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D70&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Nsa', 'FLK', 'Norte de Santander');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('54', 'COL', 'Norte de Santander');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1000</v>
       </c>
       <c r="B25" t="s">
         <v>1001</v>
       </c>
-      <c r="C25" t="s">
-        <v>1042</v>
+      <c r="C25">
+        <v>86</v>
       </c>
       <c r="D25" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D71&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Put', 'FRO', 'Putumayo');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('86', 'COL', 'Putumayo');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1002</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
-      <c r="C26" t="s">
-        <v>1043</v>
+      <c r="C26">
+        <v>63</v>
       </c>
       <c r="D26" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D72&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Qui', 'FJI', 'Quindío');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('63', 'COL', 'Quindío');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1003</v>
       </c>
       <c r="B27" t="s">
         <v>1004</v>
       </c>
-      <c r="C27" t="s">
-        <v>1044</v>
+      <c r="C27">
+        <v>66</v>
       </c>
       <c r="D27" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D73&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Ris', 'FIN', 'Risaralda');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('66', 'COL', 'Risaralda');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1005</v>
       </c>
       <c r="B28" t="s">
         <v>1006</v>
       </c>
-      <c r="C28" t="s">
-        <v>1045</v>
+      <c r="C28">
+        <v>88</v>
       </c>
       <c r="D28" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D74&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Sap', 'FRA', 'San Andrés y Providencia');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('88', 'COL', 'San Andrés y Providencia');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1007</v>
       </c>
       <c r="B29" t="s">
         <v>1008</v>
       </c>
-      <c r="C29" t="s">
-        <v>1046</v>
+      <c r="C29">
+        <v>68</v>
       </c>
       <c r="D29" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D75&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('San', 'PYF', 'Santander');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('68', 'COL', 'Santander');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1009</v>
       </c>
       <c r="B30" t="s">
         <v>1010</v>
       </c>
-      <c r="C30" t="s">
-        <v>1047</v>
+      <c r="C30">
+        <v>70</v>
       </c>
       <c r="D30" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D76&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Suc', 'GAB', 'Sucre');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('70', 'COL', 'Sucre');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1011</v>
       </c>
       <c r="B31" t="s">
         <v>1012</v>
       </c>
-      <c r="C31" t="s">
-        <v>1048</v>
+      <c r="C31">
+        <v>73</v>
       </c>
       <c r="D31" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D77&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Tol', 'GMB', 'Tolima');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('73', 'COL', 'Tolima');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1013</v>
       </c>
       <c r="B32" t="s">
         <v>1014</v>
       </c>
-      <c r="C32" t="s">
-        <v>1049</v>
+      <c r="C32">
+        <v>76</v>
       </c>
       <c r="D32" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D78&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Vac', 'GEO', 'Valle del Cauca');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('76', 'COL', 'Valle del Cauca');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1015</v>
       </c>
       <c r="B33" t="s">
         <v>1016</v>
       </c>
-      <c r="C33" t="s">
-        <v>1050</v>
+      <c r="C33">
+        <v>97</v>
       </c>
       <c r="D33" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D79&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Vau', 'DEU', 'Vaupés');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('97', 'COL', 'Vaupés');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1017</v>
       </c>
       <c r="B34" t="s">
         <v>1018</v>
       </c>
-      <c r="C34" t="s">
-        <v>1051</v>
+      <c r="C34">
+        <v>99</v>
       </c>
       <c r="D34" t="str">
-        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!D80&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('Vic', 'GHA', 'Vichada');</v>
+        <f>"INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[ID_dep]]&amp;"', '"&amp;PAIS!$D$48&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales[[#This Row],[Departamento]]&amp;"');"</f>
+        <v>INSERT INTO DEPARTAMENTO (ID_DEPARTAMENTO, ID_PAISE, NOMBRE)VALUES ('99', 'COL', 'Vichada');</v>
       </c>
     </row>
   </sheetData>
@@ -8673,523 +8496,523 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4F9882-1464-4B41-B6B0-681DD22797E1}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.296875" customWidth="1"/>
+    <col min="4" max="4" width="24.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>955</v>
       </c>
       <c r="B1" t="s">
-        <v>1053</v>
+        <v>1020</v>
       </c>
       <c r="C1" t="s">
-        <v>1052</v>
+        <v>1019</v>
       </c>
       <c r="D1" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>957</v>
       </c>
       <c r="B2" t="s">
         <v>958</v>
       </c>
-      <c r="C2" t="s">
-        <v>1054</v>
+      <c r="C2">
+        <v>91001</v>
       </c>
       <c r="D2" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Let', 'Amazonas', 'Leticia');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('91001', 'Amazonas', 'Leticia');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>959</v>
       </c>
       <c r="B3" t="s">
         <v>960</v>
       </c>
-      <c r="C3" t="s">
-        <v>1055</v>
+      <c r="C3">
+        <v>5001</v>
       </c>
       <c r="D3" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Med', 'Antioquia', 'Medellín');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('5001', 'Antioquia', 'Medellín');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>961</v>
       </c>
       <c r="B4" t="s">
         <v>961</v>
       </c>
-      <c r="C4" t="s">
-        <v>1021</v>
+      <c r="C4">
+        <v>81001</v>
       </c>
       <c r="D4" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Ara', 'Arauca', 'Arauca');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('81001', 'Arauca', 'Arauca');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>962</v>
       </c>
       <c r="B5" t="s">
         <v>963</v>
       </c>
-      <c r="C5" t="s">
-        <v>1056</v>
+      <c r="C5">
+        <v>8001</v>
       </c>
       <c r="D5" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Bar', 'Atlántico', 'Barranquilla');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('8001', 'Atlántico', 'Barranquilla');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>964</v>
       </c>
       <c r="B6" t="s">
         <v>964</v>
       </c>
-      <c r="C6" t="s">
-        <v>1023</v>
+      <c r="C6">
+        <v>11001</v>
       </c>
       <c r="D6" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Bog', 'Bogotá', 'Bogotá');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('11001', 'Bogotá', 'Bogotá');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>965</v>
       </c>
       <c r="B7" t="s">
         <v>966</v>
       </c>
-      <c r="C7" t="s">
-        <v>1057</v>
+      <c r="C7">
+        <v>13001</v>
       </c>
       <c r="D7" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Cart', 'Bolívar', 'Cartagena de Indias');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('13001', 'Bolívar', 'Cartagena de Indias');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>967</v>
       </c>
       <c r="B8" t="s">
         <v>968</v>
       </c>
-      <c r="C8" t="s">
-        <v>1058</v>
+      <c r="C8">
+        <v>15001</v>
       </c>
       <c r="D8" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Tun', 'Boyacá', 'Tunja');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('15001', 'Boyacá', 'Tunja');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>969</v>
       </c>
       <c r="B9" t="s">
         <v>970</v>
       </c>
-      <c r="C9" t="s">
-        <v>1059</v>
+      <c r="C9">
+        <v>17001</v>
       </c>
       <c r="D9" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Man', 'Caldas', 'Manizales');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('17001', 'Caldas', 'Manizales');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>971</v>
       </c>
       <c r="B10" t="s">
         <v>972</v>
       </c>
-      <c r="C10" t="s">
-        <v>1060</v>
+      <c r="C10">
+        <v>18001</v>
       </c>
       <c r="D10" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Flo', 'Caquetá', 'Florencia');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('18001', 'Caquetá', 'Florencia');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>973</v>
       </c>
       <c r="B11" t="s">
         <v>974</v>
       </c>
-      <c r="C11" t="s">
-        <v>1061</v>
+      <c r="C11">
+        <v>85001</v>
       </c>
       <c r="D11" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Yop', 'Casanare', 'Yopal');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('85001', 'Casanare', 'Yopal');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>975</v>
       </c>
       <c r="B12" t="s">
         <v>976</v>
       </c>
-      <c r="C12" t="s">
-        <v>1062</v>
+      <c r="C12">
+        <v>19001</v>
       </c>
       <c r="D12" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Pop', 'Cauca', 'Popayán');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('19001', 'Cauca', 'Popayán');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>977</v>
       </c>
       <c r="B13" t="s">
         <v>978</v>
       </c>
-      <c r="C13" t="s">
-        <v>1063</v>
+      <c r="C13">
+        <v>20001</v>
       </c>
       <c r="D13" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Vap', 'Cesar', 'Valledupar');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('20001', 'Cesar', 'Valledupar');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>979</v>
       </c>
       <c r="B14" t="s">
         <v>980</v>
       </c>
-      <c r="C14" t="s">
-        <v>1064</v>
+      <c r="C14">
+        <v>27001</v>
       </c>
       <c r="D14" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Qd', 'Chocó', 'Quibdó');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('27001', 'Chocó', 'Quibdó');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>981</v>
       </c>
       <c r="B15" t="s">
         <v>982</v>
       </c>
-      <c r="C15" t="s">
-        <v>1065</v>
+      <c r="C15">
+        <v>23001</v>
       </c>
       <c r="D15" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Mon', 'Córdoba', 'Montería');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('23001', 'Córdoba', 'Montería');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>983</v>
       </c>
       <c r="B16" t="s">
-        <v>964</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1023</v>
+        <v>1022</v>
+      </c>
+      <c r="C16">
+        <v>25001</v>
       </c>
       <c r="D16" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Bog', 'Cundinamarca', 'Bogotá');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('25001', 'Cundinamarca', 'Agua de dios');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>984</v>
       </c>
       <c r="B17" t="s">
         <v>985</v>
       </c>
-      <c r="C17" t="s">
-        <v>1066</v>
+      <c r="C17">
+        <v>94001</v>
       </c>
       <c r="D17" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Iní', 'Guainía', 'Inírida');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('94001', 'Guainía', 'Inírida');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>986</v>
       </c>
       <c r="B18" t="s">
         <v>987</v>
       </c>
-      <c r="C18" t="s">
-        <v>1067</v>
+      <c r="C18">
+        <v>95001</v>
       </c>
       <c r="D18" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('SJG', 'Guaviare', 'San José del Guaviare');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('95001', 'Guaviare', 'San José del Guaviare');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>988</v>
       </c>
       <c r="B19" t="s">
         <v>989</v>
       </c>
-      <c r="C19" t="s">
-        <v>1068</v>
+      <c r="C19">
+        <v>41001</v>
       </c>
       <c r="D19" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Nei', 'Huila', 'Neiva');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('41001', 'Huila', 'Neiva');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>990</v>
       </c>
       <c r="B20" t="s">
         <v>991</v>
       </c>
-      <c r="C20" t="s">
-        <v>1069</v>
+      <c r="C20">
+        <v>44001</v>
       </c>
       <c r="D20" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Rio', 'La Guajira', 'Riohacha');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('44001', 'La Guajira', 'Riohacha');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>992</v>
       </c>
       <c r="B21" t="s">
         <v>993</v>
       </c>
-      <c r="C21" t="s">
-        <v>1070</v>
+      <c r="C21">
+        <v>47001</v>
       </c>
       <c r="D21" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Sam', 'Magdalena', 'Santa Marta');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('47001', 'Magdalena', 'Santa Marta');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>994</v>
       </c>
       <c r="B22" t="s">
         <v>995</v>
       </c>
-      <c r="C22" t="s">
-        <v>1071</v>
+      <c r="C22">
+        <v>50001</v>
       </c>
       <c r="D22" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Viv', 'Meta', 'Villavicencio');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('50001', 'Meta', 'Villavicencio');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>996</v>
       </c>
       <c r="B23" t="s">
         <v>997</v>
       </c>
-      <c r="C23" t="s">
-        <v>1072</v>
+      <c r="C23">
+        <v>52001</v>
       </c>
       <c r="D23" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Pas', 'Nariño', 'Pasto');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('52001', 'Nariño', 'Pasto');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>998</v>
       </c>
       <c r="B24" t="s">
-        <v>999</v>
-      </c>
-      <c r="C24" t="s">
-        <v>999</v>
+        <v>1021</v>
+      </c>
+      <c r="C24">
+        <v>54001</v>
       </c>
       <c r="D24" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('San José de Cúcuta', 'Norte de Santander', 'San José de Cúcuta');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('54001', 'Norte de Santander', ' Cúcuta');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1000</v>
       </c>
       <c r="B25" t="s">
         <v>1001</v>
       </c>
-      <c r="C25" t="s">
-        <v>1073</v>
+      <c r="C25">
+        <v>86001</v>
       </c>
       <c r="D25" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Moc', 'Putumayo', 'Mocoa');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('86001', 'Putumayo', 'Mocoa');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1002</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
-      <c r="C26" t="s">
-        <v>1074</v>
+      <c r="C26">
+        <v>63001</v>
       </c>
       <c r="D26" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Arm', 'Quindío', 'Armenia');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('63001', 'Quindío', 'Armenia');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1003</v>
       </c>
       <c r="B27" t="s">
         <v>1004</v>
       </c>
-      <c r="C27" t="s">
-        <v>1075</v>
+      <c r="C27">
+        <v>66001</v>
       </c>
       <c r="D27" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Per', 'Risaralda', 'Pereira');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('66001', 'Risaralda', 'Pereira');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1005</v>
       </c>
       <c r="B28" t="s">
         <v>1006</v>
       </c>
-      <c r="C28" t="s">
-        <v>1076</v>
+      <c r="C28">
+        <v>88001</v>
       </c>
       <c r="D28" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Sad', 'San Andrés y Providencia', 'San Andrés');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('88001', 'San Andrés y Providencia', 'San Andrés');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1007</v>
       </c>
       <c r="B29" t="s">
         <v>1008</v>
       </c>
-      <c r="C29" t="s">
-        <v>1077</v>
+      <c r="C29">
+        <v>68001</v>
       </c>
       <c r="D29" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Buc', 'Santander', 'Bucaramanga');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('68001', 'Santander', 'Bucaramanga');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1009</v>
       </c>
       <c r="B30" t="s">
         <v>1010</v>
       </c>
-      <c r="C30" t="s">
-        <v>1078</v>
+      <c r="C30">
+        <v>70001</v>
       </c>
       <c r="D30" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Sinc', 'Sucre', 'Sincelejo');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('70001', 'Sucre', 'Sincelejo');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1011</v>
       </c>
       <c r="B31" t="s">
         <v>1012</v>
       </c>
-      <c r="C31" t="s">
-        <v>1079</v>
+      <c r="C31">
+        <v>73001</v>
       </c>
       <c r="D31" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Iba', 'Tolima', 'Ibagué');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('73001', 'Tolima', 'Ibagué');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1013</v>
       </c>
       <c r="B32" t="s">
         <v>1014</v>
       </c>
-      <c r="C32" t="s">
-        <v>1026</v>
+      <c r="C32">
+        <v>76001</v>
       </c>
       <c r="D32" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Cal', 'Valle del Cauca', 'Cali');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('76001', 'Valle del Cauca', 'Cali');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1015</v>
       </c>
       <c r="B33" t="s">
         <v>1016</v>
       </c>
-      <c r="C33" t="s">
-        <v>1080</v>
+      <c r="C33">
+        <v>97001</v>
       </c>
       <c r="D33" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Mit', 'Vaupés', 'Mitú');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('97001', 'Vaupés', 'Mitú');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1017</v>
       </c>
       <c r="B34" t="s">
         <v>1018</v>
       </c>
-      <c r="C34" t="s">
-        <v>1081</v>
+      <c r="C34">
+        <v>99001</v>
       </c>
       <c r="D34" t="str">
         <f>"INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[ID_dep]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Departamento]]&amp;"', '"&amp;Lista_de_todos_los_departamentos_de_Colombia_y_sus_capitales4[[#This Row],[Ciudad_Capital]]&amp;"');"</f>
-        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('Ptc', 'Vichada', 'Puerto Carreño');</v>
+        <v>INSERT INTO DEPARTAMENTO (ID_CIUDAD, ID_DPTO, NOMBRE)VALUES ('99001', 'Vichada', 'Puerto Carreño');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>